<commit_message>
increasing initial share nitrate:amino_acids in the roots as it seems to be closer to the stady-state of the model.
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -1538,8 +1538,8 @@
   </sheetPr>
   <dimension ref="A1:AY66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P17" workbookViewId="0">
-      <selection activeCell="AC50" sqref="AC50"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8078,15 +8078,15 @@
       </c>
       <c r="E49" s="28">
         <f>E50*$K$49</f>
-        <v>157.02970067046741</v>
+        <v>157.926356766808</v>
       </c>
       <c r="F49" s="28">
         <f>F50*$K$49</f>
-        <v>7.8369089556621496</v>
+        <v>2.1495432353297694</v>
       </c>
       <c r="G49" s="28">
         <f>G50*$K$49</f>
-        <v>15.673817911324299</v>
+        <v>21.495432353297694</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>32</v>
@@ -8099,15 +8099,15 @@
       </c>
       <c r="K49" s="1">
         <f>$P$55/$O$50/(1+$E$50*$E$53+$F$50*$F$53+$G$50*$G$53)</f>
-        <v>3.559339881863928E-2</v>
+        <v>3.5796640867143147E-2</v>
       </c>
       <c r="L49" s="28">
         <f>K49*$Y$38</f>
-        <v>1.779669940931964E-4</v>
+        <v>1.7898320433571574E-4</v>
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>0.17796699409319638</v>
+        <v>0.17898320433571574</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -8145,11 +8145,11 @@
       </c>
       <c r="F50" s="58">
         <f>(($Q$50/100)*(1+$E$50*$E$53)-$Y$38)/((1+1/$P$50)*(14*10^-6-$J$53*$Q$50/100))</f>
-        <v>220.17871896960222</v>
+        <v>60.04874153716424</v>
       </c>
       <c r="G50" s="58">
         <f>F50/$P$50</f>
-        <v>440.35743793920443</v>
+        <v>600.48741537164233</v>
       </c>
       <c r="H50" s="21"/>
       <c r="I50" s="21"/>
@@ -8161,7 +8161,7 @@
       </c>
       <c r="N50" s="77">
         <f>SUM(AJ5:AJ12,J37:J42)/K49</f>
-        <v>0.56505870245862833</v>
+        <v>0.56185047717741099</v>
       </c>
       <c r="O50" s="16">
         <f>INPUTS!O28</f>
@@ -8169,7 +8169,7 @@
       </c>
       <c r="P50" s="16">
         <f>INPUTS!P28</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="Q50" s="16">
         <f>INPUTS!Q28</f>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="P52" s="36">
         <f>K49+SUM(J37:J42)+SUM(AJ5:AJ34)</f>
-        <v>5.660205295951682E-2</v>
+        <v>5.6805295008020687E-2</v>
       </c>
       <c r="R52" s="95"/>
       <c r="S52" s="9" t="s">
@@ -8552,7 +8552,7 @@
       </c>
       <c r="P60" s="39">
         <f>1-$K$49/$P$56</f>
-        <v>0.14979428461709776</v>
+        <v>0.14493952061648685</v>
       </c>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.25">
@@ -8664,7 +8664,7 @@
       </c>
       <c r="P62" s="39">
         <f>1-$K$49/($P$56+1/(1+N50)*P54)</f>
-        <v>0.14979428461709776</v>
+        <v>0.14493952061648685</v>
       </c>
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.25">
@@ -8716,7 +8716,7 @@
   <dimension ref="A1:AY44"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11238,15 +11238,15 @@
       </c>
       <c r="E27" s="28">
         <f>E28*$K$27</f>
-        <v>149.22338276804928</v>
+        <v>150.07546396863901</v>
       </c>
       <c r="F27" s="28">
         <f>F28*$K$27</f>
-        <v>7.4473176718540657</v>
+        <v>2.0426843559691696</v>
       </c>
       <c r="G27" s="28">
         <f>G28*$K$27</f>
-        <v>14.894635343708131</v>
+        <v>20.426843559691694</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>32</v>
@@ -11259,15 +11259,15 @@
       </c>
       <c r="K27" s="1">
         <f>$P$33/$O$28/(1+$E$28*$E$31+$F$28*$F$31+$G$28*$G$31)</f>
-        <v>3.3823966760757836E-2</v>
+        <v>3.4017105166224838E-2</v>
       </c>
       <c r="L27" s="28">
         <f>K27*$Y$16</f>
-        <v>1.6911983380378919E-4</v>
+        <v>1.7008552583112419E-4</v>
       </c>
       <c r="M27" s="28">
         <f>M28*$K$27</f>
-        <v>0.16911983380378917</v>
+        <v>0.17008552583112418</v>
       </c>
       <c r="N27" s="76" t="s">
         <v>134</v>
@@ -11305,11 +11305,11 @@
       </c>
       <c r="F28" s="58">
         <f>(($Q$28/100)*(1+$E$28*$E$31)-$Y$16)/((1+1/$P$28)*(14*10^-6-$J$31*$Q$28/100))</f>
-        <v>220.17871896960222</v>
+        <v>60.04874153716424</v>
       </c>
       <c r="G28" s="58">
         <f>F28/$P$28</f>
-        <v>440.35743793920443</v>
+        <v>600.48741537164233</v>
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -11321,13 +11321,13 @@
       </c>
       <c r="N28" s="77">
         <f>SUM(AJ5:AJ12,J15:J20)/K27</f>
-        <v>0.59691825677279609</v>
+        <v>0.59352914298007664</v>
       </c>
       <c r="O28" s="16">
         <v>0.8</v>
       </c>
       <c r="P28" s="16">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="Q28" s="16">
         <v>1.2</v>
@@ -11384,7 +11384,7 @@
       </c>
       <c r="P30" s="69">
         <f>K27+SUM(J15:J20)+SUM(AJ5:AJ12)</f>
-        <v>5.4014110036730394E-2</v>
+        <v>5.4207248442197396E-2</v>
       </c>
       <c r="R30" s="95"/>
       <c r="S30" s="9" t="s">
@@ -11506,7 +11506,7 @@
       </c>
       <c r="P34" s="36">
         <f>K27+E27*E31+F27*F31+G27*G31</f>
-        <v>3.978327379924132E-2</v>
+        <v>3.9783273799241313E-2</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11615,7 +11615,7 @@
       </c>
       <c r="P38" s="39">
         <f>1-$K$27/$P$34</f>
-        <v>0.14979428461709776</v>
+        <v>0.14493952061648674</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -11633,7 +11633,7 @@
       </c>
       <c r="P40" s="39">
         <f>1-$K$27/($P$34+1/(1+N28)*P32)</f>
-        <v>0.14979428461709776</v>
+        <v>0.14493952061648674</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correction of soil N inputs and plant density
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -1180,7 +1180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1344,6 +1344,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -17674,7 +17677,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17684,19 +17687,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="108" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="108" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="108" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="108" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="108" t="s">
         <v>164</v>
       </c>
       <c r="I1" t="s">
@@ -17708,15 +17711,15 @@
         <v>158</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <f>B2*10^3/10000</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="94">
         <f>C2*10^6/14</f>
-        <v>428571.42857142858</v>
+        <v>571428.57142857148</v>
       </c>
       <c r="E2" s="95">
         <v>36146</v>

</xml_diff>

<commit_message>
Add inputs for calculation of lamina maximum width
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="178">
   <si>
     <t>plant</t>
   </si>
@@ -1665,8 +1665,8 @@
   </sheetPr>
   <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,14 +2136,14 @@
         <f t="shared" ref="W6:W12" si="12">$W$2*EXP($X$2*E6)</f>
         <v>2.6776375833009532E-5</v>
       </c>
-      <c r="X6">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="Y6">
-        <v>18</v>
-      </c>
-      <c r="Z6">
-        <v>0.14000000000000001</v>
+      <c r="X6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>32</v>
       </c>
       <c r="AA6" t="s">
         <v>33</v>
@@ -2230,13 +2230,13 @@
         <f>$T$27+$T$28*$T$30*(J6)^$T$29</f>
         <v>9.1017858127080242E-4</v>
       </c>
-      <c r="AX6" s="9">
+      <c r="AX6" s="9" t="e">
         <f t="shared" si="7"/>
-        <v>4.0516000000000007E-3</v>
-      </c>
-      <c r="AY6" s="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY6" s="10" t="e">
         <f>((AX6-AW6)/($T$31-AV6))*(F6-$T$31)+AX6</f>
-        <v>7.9411698532703143E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AZ6" s="10">
         <f t="shared" si="8"/>
@@ -7602,7 +7602,7 @@
   <dimension ref="A1:BC66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8069,16 +8069,16 @@
       <c r="W6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X6">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="Y6">
+      <c r="X6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y6" t="str">
         <f>INPUTS!Y6</f>
-        <v>18</v>
-      </c>
-      <c r="Z6">
+        <v>NA</v>
+      </c>
+      <c r="Z6" t="str">
         <f>INPUTS!Z6</f>
-        <v>0.14000000000000001</v>
+        <v>NA</v>
       </c>
       <c r="AA6" t="s">
         <v>33</v>
@@ -8169,13 +8169,13 @@
         <f>$T$49+$T$50*$T$52*(J6)^$T$51</f>
         <v>9.1017858127080242E-4</v>
       </c>
-      <c r="AY6" s="9">
+      <c r="AY6" s="9" t="e">
         <f t="shared" si="7"/>
-        <v>4.0516000000000007E-3</v>
-      </c>
-      <c r="AZ6" s="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ6" s="10" t="e">
         <f>((AY6-AX6)/($T$53-AW6))*(F6-$T$53)+AY6</f>
-        <v>7.9411698532703143E-4</v>
+        <v>#VALUE!</v>
       </c>
       <c r="BA6" s="10">
         <f>$T$49+$T$50*0.5*(L6)^$T$51</f>
@@ -9392,17 +9392,17 @@
         <f t="shared" ref="W13" si="22">W6</f>
         <v>NA</v>
       </c>
-      <c r="X13">
-        <f t="shared" si="21"/>
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="Y13">
-        <f t="shared" si="21"/>
-        <v>18</v>
-      </c>
-      <c r="Z13">
-        <f t="shared" si="21"/>
-        <v>0.14000000000000001</v>
+      <c r="X13" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+      <c r="Y13" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+      <c r="Z13" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="21"/>

</xml_diff>

<commit_message>
- number of replication of MS on each tiller is now given as simulation option - temporary : cytokinin concentration of new tissue can be given as simulation parameter
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS" sheetId="15" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="INPUTS_save2" sheetId="9" r:id="rId4"/>
     <sheet name="Soil" sheetId="18" r:id="rId5"/>
     <sheet name="Barillot2016b_inputs" sheetId="6" r:id="rId6"/>
+    <sheet name="Bertheloot2011b" sheetId="19" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -121,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="183">
   <si>
     <t>plant</t>
   </si>
@@ -766,6 +767,21 @@
   </si>
   <si>
     <t>RER_Wmax_int</t>
+  </si>
+  <si>
+    <t>Grains</t>
+  </si>
+  <si>
+    <t>Ped_exp</t>
+  </si>
+  <si>
+    <t>Ped_enc</t>
+  </si>
+  <si>
+    <t>Roots = 15% DM Shoot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; FAUX</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1682,7 @@
   <dimension ref="A1:BB44"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4350,7 +4366,7 @@
       </c>
       <c r="M27" s="28">
         <f>M28*$K$27</f>
-        <v>0.91064195735270959</v>
+        <v>0.45532097867635479</v>
       </c>
       <c r="N27" s="76" t="s">
         <v>134</v>
@@ -4402,7 +4418,7 @@
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
       <c r="M28" s="22">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="N28" s="77">
         <f>SUM(AK5:AK12,J15:J20)/K27</f>
@@ -7601,8 +7617,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView topLeftCell="I13" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14682,7 +14698,7 @@
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>0.92578187857085392</v>
+        <v>0.46289093928542696</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -14735,7 +14751,7 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="22">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="N50" s="77">
         <f>SUM(AK5:AK34,J37:J42)/K49</f>
@@ -18004,7 +18020,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18038,15 +18054,15 @@
         <v>158</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>B2*10^3/10000</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="94">
         <f>C2*10^6/14</f>
-        <v>428571.42857142858</v>
+        <v>71428.571428571435</v>
       </c>
       <c r="E2" s="95">
         <v>36146</v>
@@ -18121,10 +18137,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18232,7 +18248,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="28">
-        <f t="shared" ref="I6:I20" si="1">G6/D6*1000</f>
+        <f t="shared" ref="I6:I22" si="1">G6/D6*1000</f>
         <v>88.888888888888886</v>
       </c>
     </row>
@@ -18544,58 +18560,117 @@
         <v>1.3513513513513513</v>
       </c>
     </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18">
+        <v>58</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="I18" s="28"/>
+    </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>157</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>15</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>210</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>1.01</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>15</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I20" s="28">
         <f t="shared" si="1"/>
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21">
+        <v>75</v>
+      </c>
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>107</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <f>0.5*1000</f>
         <v>500</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <f>0.01*1000</f>
         <v>10</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>2.5</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I22" s="28">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>168</v>
-      </c>
-      <c r="E23">
-        <f>SUM(D5:D19)/D20</f>
-        <v>2.8119999999999998</v>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25">
+        <f>SUM(D5:D21)/D22</f>
+        <v>3.29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1">
+        <f>1/0.15</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- add possibility to run caribu for an heterogeneous canopy - change blade max proteins inputs
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="183">
   <si>
     <t>plant</t>
   </si>
@@ -1681,8 +1681,8 @@
   </sheetPr>
   <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AB29" sqref="AB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3522,7 +3522,7 @@
         <v>0.16700714999999999</v>
       </c>
       <c r="R15">
-        <v>5000</v>
+        <v>4250</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -3558,7 +3558,7 @@
         <v>21</v>
       </c>
       <c r="AC15" s="15">
-        <f t="shared" ref="AC15:AC20" si="28">ROUND(X15/$AS$6*120,0)</f>
+        <f>ROUND(X15/$AS$6*120,0)</f>
         <v>57</v>
       </c>
       <c r="AD15" s="15">
@@ -3618,7 +3618,7 @@
         <v>1.7099999999999999E-3</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K20" si="29">J16*0.005</f>
+        <f t="shared" ref="K16:K20" si="28">J16*0.005</f>
         <v>8.5499999999999995E-6</v>
       </c>
       <c r="L16">
@@ -3683,7 +3683,7 @@
         <v>4411.7647058823532</v>
       </c>
       <c r="AC16" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="AC15:AC20" si="29">ROUND(X16/$AS$6*120,0)</f>
         <v>16</v>
       </c>
       <c r="AD16" s="15">
@@ -3742,7 +3742,7 @@
         <v>5.5446100000000002E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>2.7723050000000002E-5</v>
       </c>
       <c r="L17">
@@ -3769,7 +3769,7 @@
         <v>0.37703348000000003</v>
       </c>
       <c r="R17">
-        <v>5000</v>
+        <v>4250</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -3800,7 +3800,7 @@
         <v>10</v>
       </c>
       <c r="AC17" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>68</v>
       </c>
       <c r="AD17" s="15">
@@ -3845,7 +3845,7 @@
         <v>2.2800000000000003E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="L18">
@@ -3903,7 +3903,7 @@
         <v>121</v>
       </c>
       <c r="AC18" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="AD18" s="15">
@@ -3948,7 +3948,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="L19">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="AB19" s="1"/>
       <c r="AC19" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>23</v>
       </c>
       <c r="AD19" s="15">
@@ -4056,7 +4056,7 @@
         <v>4.8002499999999998E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>2.400125E-5</v>
       </c>
       <c r="L20">
@@ -4082,8 +4082,8 @@
         <f t="shared" si="25"/>
         <v>0.36001875</v>
       </c>
-      <c r="R20">
-        <v>5000</v>
+      <c r="R20" t="s">
+        <v>32</v>
       </c>
       <c r="S20">
         <v>0</v>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="AC20" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>75</v>
       </c>
       <c r="AD20" s="16">
@@ -7618,7 +7618,7 @@
   <dimension ref="A1:BC66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13826,7 +13826,7 @@
       </c>
       <c r="R37">
         <f>INPUTS!R15</f>
-        <v>5000</v>
+        <v>4250</v>
       </c>
       <c r="S37">
         <v>0</v>
@@ -14080,7 +14080,7 @@
       </c>
       <c r="R39">
         <f>INPUTS!R17</f>
-        <v>5000</v>
+        <v>4250</v>
       </c>
       <c r="S39">
         <v>0</v>
@@ -14399,9 +14399,9 @@
         <f t="shared" si="151"/>
         <v>0.33267174999999999</v>
       </c>
-      <c r="R42">
+      <c r="R42" t="str">
         <f>INPUTS!R20</f>
-        <v>5000</v>
+        <v>NA</v>
       </c>
       <c r="S42">
         <v>0</v>

</xml_diff>

<commit_message>
Correction input max_protein for blade 3 Increase initial cytokines concentration in the roots
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="183">
   <si>
     <t>plant</t>
   </si>
@@ -1681,8 +1681,8 @@
   </sheetPr>
   <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AB29" sqref="AB29"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,7 +3518,7 @@
         <v>1.9532999999999999E-4</v>
       </c>
       <c r="Q15" s="1">
-        <f t="shared" ref="Q15:Q20" si="25">J15*$AC15</f>
+        <f>J15*$AC15</f>
         <v>0.16700714999999999</v>
       </c>
       <c r="R15">
@@ -3537,7 +3537,7 @@
         <v>4.3</v>
       </c>
       <c r="W15" s="15">
-        <f t="shared" ref="W15:W20" si="26">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
+        <f t="shared" ref="W15:W20" si="25">(($V15/100)*(1+$AB$16*$E$31)-$Y$16)/(((1+1/$X$23)*(14*10^(-6)))-(($J$31/$X$23+$F$31)*$V15/100))</f>
         <v>395.90503059926971</v>
       </c>
       <c r="X15" s="15">
@@ -3551,7 +3551,7 @@
         <v>27</v>
       </c>
       <c r="AA15" s="89">
-        <f t="shared" ref="AA15:AA20" si="27">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
+        <f t="shared" ref="AA15:AA20" si="26">IF(F15="HiddenElement",$AA$22/100/(1-$X$33)*$X$32*10^6/$X$30,0)</f>
         <v>0</v>
       </c>
       <c r="AB15" s="88" t="s">
@@ -3618,7 +3618,7 @@
         <v>1.7099999999999999E-3</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K20" si="28">J16*0.005</f>
+        <f t="shared" ref="K16:K20" si="27">J16*0.005</f>
         <v>8.5499999999999995E-6</v>
       </c>
       <c r="L16">
@@ -3641,7 +3641,7 @@
         <v>2.6861000000000002E-4</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="Q15:Q20" si="28">J16*$AC16</f>
         <v>2.7359999999999999E-2</v>
       </c>
       <c r="R16">
@@ -3661,7 +3661,7 @@
         <v>1.8</v>
       </c>
       <c r="W16" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>112.73176271832151</v>
       </c>
       <c r="X16" s="15">
@@ -3675,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="AA16" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB16" s="56">
@@ -3683,7 +3683,7 @@
         <v>4411.7647058823532</v>
       </c>
       <c r="AC16" s="15">
-        <f t="shared" ref="AC15:AC20" si="29">ROUND(X16/$AS$6*120,0)</f>
+        <f t="shared" ref="AC16:AC20" si="29">ROUND(X16/$AS$6*120,0)</f>
         <v>16</v>
       </c>
       <c r="AD16" s="15">
@@ -3742,7 +3742,7 @@
         <v>5.5446100000000002E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2.7723050000000002E-5</v>
       </c>
       <c r="L17">
@@ -3765,7 +3765,7 @@
         <v>2.4106999999999999E-4</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0.37703348000000003</v>
       </c>
       <c r="R17">
@@ -3784,7 +3784,7 @@
         <v>4.8</v>
       </c>
       <c r="W17" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>469.29708428542818</v>
       </c>
       <c r="X17" s="15">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="Z17" s="28"/>
       <c r="AA17" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB17" s="53">
@@ -3845,7 +3845,7 @@
         <v>2.2800000000000003E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="L18">
@@ -3868,7 +3868,7 @@
         <v>2.4800000000000001E-4</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>5.2440000000000007E-2</v>
       </c>
       <c r="R18">
@@ -3888,7 +3888,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W18" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X18" s="15">
@@ -3896,7 +3896,7 @@
         <v>1604.0455673709137</v>
       </c>
       <c r="AA18" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>1323.5294117647056</v>
       </c>
       <c r="AB18" s="54" t="s">
@@ -3948,7 +3948,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="L19">
@@ -3971,7 +3971,7 @@
         <v>4.7099999999999998E-6</v>
       </c>
       <c r="Q19" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>9.2000000000000003E-4</v>
       </c>
       <c r="R19">
@@ -3991,7 +3991,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="W19" s="15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>160.40455673709138</v>
       </c>
       <c r="X19" s="15">
@@ -3999,7 +3999,7 @@
         <v>1604.0455673709137</v>
       </c>
       <c r="AA19" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AB19" s="1"/>
@@ -4056,7 +4056,7 @@
         <v>4.8002499999999998E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>2.400125E-5</v>
       </c>
       <c r="L20">
@@ -4079,11 +4079,11 @@
         <v>1.9201E-4</v>
       </c>
       <c r="Q20" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>0.36001875</v>
       </c>
-      <c r="R20" t="s">
-        <v>32</v>
+      <c r="R20">
+        <v>0</v>
       </c>
       <c r="S20">
         <v>0</v>
@@ -4098,7 +4098,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="W20" s="16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>516.91276575633913</v>
       </c>
       <c r="X20" s="16">
@@ -4106,7 +4106,7 @@
         <v>5169.127657563391</v>
       </c>
       <c r="AA20" s="90">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AC20" s="16">
@@ -4366,7 +4366,7 @@
       </c>
       <c r="M27" s="28">
         <f>M28*$K$27</f>
-        <v>0.34149073400726598</v>
+        <v>2.7319258720581279</v>
       </c>
       <c r="N27" s="76" t="s">
         <v>134</v>
@@ -4418,7 +4418,7 @@
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
       <c r="M28" s="22">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="N28" s="77">
         <f>SUM(AK5:AK12,J15:J20)/K27</f>
@@ -7617,8 +7617,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14399,9 +14399,9 @@
         <f t="shared" si="151"/>
         <v>0.33267174999999999</v>
       </c>
-      <c r="R42" t="str">
+      <c r="R42">
         <f>INPUTS!R20</f>
-        <v>NA</v>
+        <v>0</v>
       </c>
       <c r="S42">
         <v>0</v>
@@ -14698,7 +14698,7 @@
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>0.69433640892814052</v>
+        <v>2.7773456357125621</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -14751,7 +14751,7 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="22">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="N50" s="77">
         <f>SUM(AK5:AK34,J37:J42)/K49</f>

</xml_diff>

<commit_message>
- higher initial cytokinins concentrations in the first leaves - main script run with an heterogeneous stand (fixed random seed)
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -3641,7 +3641,7 @@
         <v>2.6861000000000002E-4</v>
       </c>
       <c r="Q16" s="1">
-        <f t="shared" ref="Q15:Q20" si="28">J16*$AC16</f>
+        <f t="shared" ref="Q16:Q20" si="28">J16*$AC16</f>
         <v>2.7359999999999999E-2</v>
       </c>
       <c r="R16">
@@ -7617,8 +7617,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
+      <selection activeCell="AC45" sqref="AC45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13822,7 +13822,7 @@
       </c>
       <c r="Q37" s="1">
         <f t="shared" ref="Q37:Q42" si="151">J37*$AC37</f>
-        <v>0.14960368542307284</v>
+        <v>0.24933947570512138</v>
       </c>
       <c r="R37">
         <f>INPUTS!R15</f>
@@ -13864,8 +13864,8 @@
         <v>21</v>
       </c>
       <c r="AC37" s="15">
-        <f t="shared" ref="AC37:AC42" si="154">ROUND(X37/$AS$6*$AC$45,0)</f>
-        <v>51</v>
+        <f>ROUND(X37/$AS$6*$AC$45,0)</f>
+        <v>85</v>
       </c>
       <c r="AD37" s="15">
         <f>J37+L37*$F$53+M37*$J$53+O37*$E$53</f>
@@ -13925,7 +13925,7 @@
         <v>1.7099999999999999E-3</v>
       </c>
       <c r="K38">
-        <f t="shared" ref="K38:K42" si="155">J38*0.005</f>
+        <f t="shared" ref="K38:K42" si="154">J38*0.005</f>
         <v>8.5499999999999995E-6</v>
       </c>
       <c r="L38">
@@ -13949,7 +13949,7 @@
       </c>
       <c r="Q38" s="1">
         <f t="shared" si="151"/>
-        <v>2.5649999999999999E-2</v>
+        <v>4.104E-2</v>
       </c>
       <c r="R38">
         <f>INPUTS!R16</f>
@@ -13992,8 +13992,8 @@
         <v>5882.3529411764703</v>
       </c>
       <c r="AC38" s="15">
-        <f t="shared" si="154"/>
-        <v>15</v>
+        <f t="shared" ref="AC37:AC42" si="155">ROUND(X38/$AS$6*$AC$45,0)</f>
+        <v>24</v>
       </c>
       <c r="AD38" s="15">
         <f t="shared" ref="AD38:AD42" si="156">J38+L38*$F$53+M38*$J$53+O38*$E$53</f>
@@ -14052,7 +14052,7 @@
         <v>5.2983708800493851E-3</v>
       </c>
       <c r="K39">
-        <f t="shared" si="155"/>
+        <f t="shared" si="154"/>
         <v>2.6491854400246927E-5</v>
       </c>
       <c r="L39">
@@ -14076,7 +14076,7 @@
       </c>
       <c r="Q39" s="1">
         <f t="shared" si="151"/>
-        <v>0.3232006236830125</v>
+        <v>0.53513545888498792</v>
       </c>
       <c r="R39">
         <f>INPUTS!R17</f>
@@ -14113,8 +14113,8 @@
         <v>10</v>
       </c>
       <c r="AC39" s="15">
-        <f t="shared" si="154"/>
-        <v>61</v>
+        <f t="shared" si="155"/>
+        <v>101</v>
       </c>
       <c r="AD39" s="15">
         <f t="shared" si="156"/>
@@ -14158,7 +14158,7 @@
         <v>2.2800000000000003E-3</v>
       </c>
       <c r="K40">
-        <f t="shared" si="155"/>
+        <f t="shared" si="154"/>
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="L40">
@@ -14182,7 +14182,7 @@
       </c>
       <c r="Q40" s="1">
         <f t="shared" si="151"/>
-        <v>4.7880000000000006E-2</v>
+        <v>7.980000000000001E-2</v>
       </c>
       <c r="R40">
         <f>INPUTS!R18</f>
@@ -14218,8 +14218,8 @@
         <v>121</v>
       </c>
       <c r="AC40" s="15">
-        <f t="shared" si="154"/>
-        <v>21</v>
+        <f t="shared" si="155"/>
+        <v>35</v>
       </c>
       <c r="AD40" s="15">
         <f t="shared" si="156"/>
@@ -14263,7 +14263,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="K41">
-        <f t="shared" si="155"/>
+        <f t="shared" si="154"/>
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="L41">
@@ -14287,7 +14287,7 @@
       </c>
       <c r="Q41" s="1">
         <f t="shared" si="151"/>
-        <v>8.4000000000000003E-4</v>
+        <v>1.4000000000000002E-3</v>
       </c>
       <c r="R41">
         <f>INPUTS!R19</f>
@@ -14321,8 +14321,8 @@
       </c>
       <c r="AB41" s="1"/>
       <c r="AC41" s="15">
-        <f t="shared" si="154"/>
-        <v>21</v>
+        <f t="shared" si="155"/>
+        <v>35</v>
       </c>
       <c r="AD41" s="15">
         <f t="shared" si="156"/>
@@ -14373,7 +14373,7 @@
         <v>4.96525E-3</v>
       </c>
       <c r="K42">
-        <f t="shared" si="155"/>
+        <f t="shared" si="154"/>
         <v>2.482625E-5</v>
       </c>
       <c r="L42">
@@ -14397,7 +14397,7 @@
       </c>
       <c r="Q42" s="1">
         <f t="shared" si="151"/>
-        <v>0.33267174999999999</v>
+        <v>0.55114275000000001</v>
       </c>
       <c r="R42">
         <f>INPUTS!R20</f>
@@ -14430,8 +14430,8 @@
         <v>0</v>
       </c>
       <c r="AC42" s="16">
-        <f t="shared" si="154"/>
-        <v>67</v>
+        <f t="shared" si="155"/>
+        <v>111</v>
       </c>
       <c r="AD42" s="16">
         <f t="shared" si="156"/>
@@ -14514,7 +14514,7 @@
         <v>121</v>
       </c>
       <c r="AC45" s="101">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="AN45" s="91"/>
       <c r="AO45" s="91"/>

</xml_diff>

<commit_message>
Cgange initial cytokinins concentration in the roots and initial max_proteins of leaves 1 and 2
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -7618,7 +7618,7 @@
   <dimension ref="A1:BC66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
-      <selection activeCell="AC45" sqref="AC45"/>
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13825,8 +13825,7 @@
         <v>0.24933947570512138</v>
       </c>
       <c r="R37">
-        <f>INPUTS!R15</f>
-        <v>4250</v>
+        <v>4400</v>
       </c>
       <c r="S37">
         <v>0</v>
@@ -13992,7 +13991,7 @@
         <v>5882.3529411764703</v>
       </c>
       <c r="AC38" s="15">
-        <f t="shared" ref="AC37:AC42" si="155">ROUND(X38/$AS$6*$AC$45,0)</f>
+        <f t="shared" ref="AC38:AC42" si="155">ROUND(X38/$AS$6*$AC$45,0)</f>
         <v>24</v>
       </c>
       <c r="AD38" s="15">
@@ -14079,8 +14078,7 @@
         <v>0.53513545888498792</v>
       </c>
       <c r="R39">
-        <f>INPUTS!R17</f>
-        <v>4250</v>
+        <v>4400</v>
       </c>
       <c r="S39">
         <v>0</v>
@@ -14698,7 +14696,7 @@
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>2.7773456357125621</v>
+        <v>3.4716820446407026</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -14751,7 +14749,7 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="22">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="N50" s="77">
         <f>SUM(AK5:AK34,J37:J42)/K49</f>

</xml_diff>

<commit_message>
Change in inputs (SSLW); Add option to send different parameters values to CNWheat via cnwheat_facade
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -1682,7 +1682,7 @@
   <dimension ref="A1:BB44"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,7 +1972,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="Y5">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Z5">
         <v>0.09</v>
@@ -3492,19 +3492,19 @@
       </c>
       <c r="J15">
         <f>P15*$U$15</f>
-        <v>2.9299499999999997E-3</v>
+        <v>4.2972599999999998E-3</v>
       </c>
       <c r="K15">
         <f>J15*0.005</f>
-        <v>1.464975E-5</v>
+        <v>2.1486299999999998E-5</v>
       </c>
       <c r="L15">
         <f>J15*$W15</f>
-        <v>1.1599819444043302</v>
+        <v>1.7013068517930177</v>
       </c>
       <c r="M15">
         <f t="shared" ref="M15:M20" si="22">J15*$X15</f>
-        <v>11.599819444043302</v>
+        <v>17.013068517930176</v>
       </c>
       <c r="N15">
         <f t="shared" ref="N15:N20" si="23">AA15*$J15</f>
@@ -3512,14 +3512,14 @@
       </c>
       <c r="O15" s="1">
         <f t="shared" ref="O15:O20" si="24">J15*$AB$16</f>
-        <v>12.92625</v>
+        <v>18.958500000000001</v>
       </c>
       <c r="P15">
         <v>1.9532999999999999E-4</v>
       </c>
       <c r="Q15" s="1">
         <f>J15*$AC15</f>
-        <v>0.16700714999999999</v>
+        <v>0.24494381999999998</v>
       </c>
       <c r="R15">
         <v>4250</v>
@@ -3531,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="U15" s="15">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="V15" s="15">
         <v>4.3</v>
@@ -3563,11 +3563,11 @@
       </c>
       <c r="AD15" s="15">
         <f>J15+L15*$F$31+M15*$J$31+O15*$E$31</f>
-        <v>4.4950458008899278E-3</v>
+        <v>6.5927338413052268E-3</v>
       </c>
       <c r="AE15" s="71">
         <f>(1-J15/AD15)*100</f>
-        <v>34.818239239744145</v>
+        <v>34.81823923974413</v>
       </c>
       <c r="AF15" s="1"/>
       <c r="AO15" s="82"/>
@@ -3739,19 +3739,19 @@
       </c>
       <c r="J17">
         <f>P17*$U$17</f>
-        <v>5.5446100000000002E-3</v>
+        <v>5.3035399999999998E-3</v>
       </c>
       <c r="K17">
         <f t="shared" si="27"/>
-        <v>2.7723050000000002E-5</v>
+        <v>2.6517699999999999E-5</v>
       </c>
       <c r="L17">
         <f t="shared" ref="L17:L20" si="32">J17*$W17</f>
-        <v>2.6020693064998279</v>
+        <v>2.4889358583911396</v>
       </c>
       <c r="M17">
         <f t="shared" si="22"/>
-        <v>26.02069306499828</v>
+        <v>24.889358583911395</v>
       </c>
       <c r="N17">
         <f t="shared" si="23"/>
@@ -3759,14 +3759,14 @@
       </c>
       <c r="O17" s="1">
         <f t="shared" si="24"/>
-        <v>24.461514705882355</v>
+        <v>23.397970588235296</v>
       </c>
       <c r="P17">
         <v>2.4106999999999999E-4</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="28"/>
-        <v>0.37703348000000003</v>
+        <v>0.36064071999999997</v>
       </c>
       <c r="R17">
         <v>4250</v>
@@ -3778,7 +3778,7 @@
         <v>0</v>
       </c>
       <c r="U17" s="15">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V17" s="15">
         <v>4.8</v>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="AD17" s="15">
         <f t="shared" si="30"/>
-        <v>8.9258692333536154E-3</v>
+        <v>8.5377879623382402E-3</v>
       </c>
       <c r="AE17" s="71">
         <f t="shared" si="31"/>
@@ -4053,19 +4053,19 @@
       </c>
       <c r="J20">
         <f>P20*$U$20</f>
-        <v>4.8002499999999998E-3</v>
+        <v>4.2242199999999999E-3</v>
       </c>
       <c r="K20">
         <f t="shared" si="27"/>
-        <v>2.400125E-5</v>
+        <v>2.11211E-5</v>
       </c>
       <c r="L20">
         <f t="shared" si="32"/>
-        <v>2.481310503821867</v>
+        <v>2.1835532433632427</v>
       </c>
       <c r="M20">
         <f t="shared" si="22"/>
-        <v>24.813105038218666</v>
+        <v>21.835532433632427</v>
       </c>
       <c r="N20">
         <f t="shared" si="23"/>
@@ -4073,14 +4073,14 @@
       </c>
       <c r="O20" s="1">
         <f t="shared" si="24"/>
-        <v>21.177573529411767</v>
+        <v>18.636264705882354</v>
       </c>
       <c r="P20">
         <v>1.9201E-4</v>
       </c>
       <c r="Q20" s="1">
         <f t="shared" si="28"/>
-        <v>0.36001875</v>
+        <v>0.3168165</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -4092,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="16">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="V20" s="16">
         <v>5.0999999999999996</v>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="AD20" s="16">
         <f t="shared" si="30"/>
-        <v>7.9631974036974019E-3</v>
+        <v>7.0076137152537141E-3</v>
       </c>
       <c r="AE20" s="72">
         <f t="shared" si="31"/>
@@ -4183,7 +4183,7 @@
       </c>
       <c r="Y23" s="74">
         <f>(SUMPRODUCT(V15:V20,AD15:AD20)+SUMPRODUCT(AQ5:AQ12,AO5:AO12))/SUM(AD15:AD20,AO5:AO12)</f>
-        <v>4.4477344970038697</v>
+        <v>4.4146203981518433</v>
       </c>
       <c r="AA23" s="54" t="s">
         <v>121</v>
@@ -4337,15 +4337,15 @@
       </c>
       <c r="E27" s="28">
         <f>E28*$K$27</f>
-        <v>150.65767676791148</v>
+        <v>154.21320252380491</v>
       </c>
       <c r="F27" s="28">
         <f>F28*$K$27</f>
-        <v>2.0506088823738819</v>
+        <v>2.0990033143932734</v>
       </c>
       <c r="G27" s="28">
         <f>G28*$K$27</f>
-        <v>20.506088823738818</v>
+        <v>20.990033143932731</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>32</v>
@@ -4358,15 +4358,15 @@
       </c>
       <c r="K27" s="1">
         <f>$P$33/$O$28/(1+$E$28*$E$31+$F$28*$F$31+$G$28*$G$31)</f>
-        <v>3.41490734007266E-2</v>
+        <v>3.4954992572062443E-2</v>
       </c>
       <c r="L27" s="28">
         <f>K27*$Y$16</f>
-        <v>1.70745367003633E-4</v>
+        <v>1.7477496286031222E-4</v>
       </c>
       <c r="M27" s="28">
         <f>M28*$K$27</f>
-        <v>2.7319258720581279</v>
+        <v>2.7963994057649955</v>
       </c>
       <c r="N27" s="76" t="s">
         <v>134</v>
@@ -4422,7 +4422,7 @@
       </c>
       <c r="N28" s="77">
         <f>SUM(AK5:AK12,J15:J20)/K27</f>
-        <v>0.59123546454829934</v>
+        <v>0.59334451961947088</v>
       </c>
       <c r="O28" s="16">
         <v>0.8</v>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="P30" s="69">
         <f>K27+SUM(J15:J20)+SUM(AK5:AK12)</f>
-        <v>5.4339216676699158E-2</v>
+        <v>5.5695345848035004E-2</v>
       </c>
       <c r="R30" s="110"/>
       <c r="S30" s="9" t="s">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="P33" s="69">
         <f t="array" ref="P33">SUM(J15:J20,AK5:AK12)+SUM(AF5:AF12*F31,L15:L20*F31)+SUM(AH5:AH12*J31,M15:M20*J31)+SUM(AE5:AE12*E31,O15:O20*E31)+SUM(N15:N20*E31,AG5:AG12*E31)</f>
-        <v>3.1950089355408044E-2</v>
+        <v>3.2704112436364279E-2</v>
       </c>
       <c r="W33" s="35" t="s">
         <v>122</v>
@@ -4615,7 +4615,7 @@
       </c>
       <c r="P34" s="36">
         <f>K27+E27*E31+F27*F31+G27*G31</f>
-        <v>3.9937611694260043E-2</v>
+        <v>4.0880140545455336E-2</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="P35" s="36">
         <f>P34+P33+P32</f>
-        <v>7.1887701049668087E-2</v>
+        <v>7.3584252981819614E-2</v>
       </c>
       <c r="Q35" s="32"/>
     </row>
@@ -4715,7 +4715,7 @@
       </c>
       <c r="P37" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$15:$J$20)/$P$33</f>
-        <v>0.36807240031849642</v>
+        <v>0.36581818826824364</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="P38" s="39">
         <f>1-$K$27/$P$34</f>
-        <v>0.14493952061648674</v>
+        <v>0.14493952061648663</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="P39" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$15:$J$20)/($P$33+N28/(1+N28)*P32)</f>
-        <v>0.36807240031849642</v>
+        <v>0.36581818826824364</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -4742,7 +4742,7 @@
       </c>
       <c r="P40" s="39">
         <f>1-$K$27/($P$34+1/(1+N28)*P32)</f>
-        <v>0.14493952061648674</v>
+        <v>0.14493952061648663</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="P44" s="75">
         <f>($Y$23*$P$33+$Q$28*$P$34)/($P$33+$P$34)</f>
-        <v>2.6434375542239423</v>
+        <v>2.6287201769563748</v>
       </c>
     </row>
   </sheetData>
@@ -7617,8 +7617,8 @@
   </sheetPr>
   <dimension ref="A1:BC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7901,7 +7901,7 @@
       </c>
       <c r="Y5">
         <f>INPUTS!Y5</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Z5">
         <f>INPUTS!Z5</f>
@@ -13795,19 +13795,19 @@
       </c>
       <c r="J37">
         <f>P37*$U$37</f>
-        <v>2.93340559653084E-3</v>
+        <v>4.3023282082452321E-3</v>
       </c>
       <c r="K37">
         <f>J37*0.005</f>
-        <v>1.46670279826542E-5</v>
+        <v>2.1511641041226162E-5</v>
       </c>
       <c r="L37">
         <f>J37*$W37</f>
-        <v>1.2096740612871526</v>
+        <v>1.7741886232211572</v>
       </c>
       <c r="M37">
         <f t="shared" ref="M37:M42" si="148">J37*$X37</f>
-        <v>12.096740612871526</v>
+        <v>17.74188623221157</v>
       </c>
       <c r="N37">
         <f t="shared" ref="N37:N42" si="149">AA37*$J37</f>
@@ -13815,14 +13815,14 @@
       </c>
       <c r="O37" s="1">
         <f t="shared" ref="O37:O42" si="150">J37*$AB$38</f>
-        <v>17.255327038416706</v>
+        <v>25.307812989677835</v>
       </c>
       <c r="P37">
         <v>1.9556037310205601E-4</v>
       </c>
       <c r="Q37" s="1">
         <f t="shared" ref="Q37:Q42" si="151">J37*$AC37</f>
-        <v>0.24933947570512138</v>
+        <v>0.36569789770084471</v>
       </c>
       <c r="R37">
         <v>4400</v>
@@ -13835,7 +13835,7 @@
       </c>
       <c r="U37" s="15">
         <f>INPUTS!U15</f>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="V37" s="15">
         <f>INPUTS!V15</f>
@@ -13868,7 +13868,7 @@
       </c>
       <c r="AD37" s="15">
         <f>J37+L37*$F$53+M37*$J$53+O37*$E$53</f>
-        <v>4.6734147307180398E-3</v>
+        <v>6.8543416050531256E-3</v>
       </c>
       <c r="AE37" s="71">
         <f>(1-J37/AD37)*100</f>
@@ -14048,19 +14048,19 @@
       </c>
       <c r="J39">
         <f>P39*$U$39</f>
-        <v>5.2983708800493851E-3</v>
+        <v>5.0680069287428898E-3</v>
       </c>
       <c r="K39">
         <f t="shared" si="154"/>
-        <v>2.6491854400246927E-5</v>
+        <v>2.5340034643714449E-5</v>
       </c>
       <c r="L39">
         <f t="shared" ref="L39:L42" si="158">J39*$W39</f>
-        <v>2.5887478676102722</v>
+        <v>2.4761936124967816</v>
       </c>
       <c r="M39">
         <f t="shared" si="148"/>
-        <v>25.887478676102717</v>
+        <v>24.761936124967814</v>
       </c>
       <c r="N39">
         <f t="shared" si="149"/>
@@ -14068,14 +14068,14 @@
       </c>
       <c r="O39" s="1">
         <f t="shared" si="150"/>
-        <v>31.166887529702265</v>
+        <v>29.811805463193469</v>
       </c>
       <c r="P39">
         <v>2.3036395130649501E-4</v>
       </c>
       <c r="Q39" s="1">
         <f t="shared" si="151"/>
-        <v>0.53513545888498792</v>
+        <v>0.51186869980303185</v>
       </c>
       <c r="R39">
         <v>4400</v>
@@ -14088,7 +14088,7 @@
       </c>
       <c r="U39" s="15">
         <f>INPUTS!U17</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V39" s="15">
         <f>INPUTS!V17</f>
@@ -14116,7 +14116,7 @@
       </c>
       <c r="AD39" s="15">
         <f t="shared" si="156"/>
-        <v>8.8574797085881011E-3</v>
+        <v>8.4723718951712264E-3</v>
       </c>
       <c r="AE39" s="71">
         <f t="shared" si="157"/>
@@ -14368,19 +14368,19 @@
       </c>
       <c r="J42">
         <f>P42*$U$42</f>
-        <v>4.96525E-3</v>
+        <v>4.3694199999999997E-3</v>
       </c>
       <c r="K42">
         <f t="shared" si="154"/>
-        <v>2.482625E-5</v>
+        <v>2.18471E-5</v>
       </c>
       <c r="L42">
         <f t="shared" si="158"/>
-        <v>2.6715030629034748</v>
+        <v>2.3509226953550577</v>
       </c>
       <c r="M42">
         <f t="shared" si="148"/>
-        <v>26.715030629034747</v>
+        <v>23.509226953550574</v>
       </c>
       <c r="N42">
         <f t="shared" si="149"/>
@@ -14388,14 +14388,14 @@
       </c>
       <c r="O42" s="1">
         <f t="shared" si="150"/>
-        <v>29.20735294117647</v>
+        <v>25.70247058823529</v>
       </c>
       <c r="P42">
         <v>1.9861E-4</v>
       </c>
       <c r="Q42" s="1">
         <f t="shared" si="151"/>
-        <v>0.55114275000000001</v>
+        <v>0.48500561999999997</v>
       </c>
       <c r="R42">
         <f>INPUTS!R20</f>
@@ -14409,7 +14409,7 @@
       </c>
       <c r="U42" s="16">
         <f>INPUTS!U20</f>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="V42" s="16">
         <f>INPUTS!V20</f>
@@ -14433,7 +14433,7 @@
       </c>
       <c r="AD42" s="16">
         <f t="shared" si="156"/>
-        <v>8.5536808173948056E-3</v>
+        <v>7.5272391193074283E-3</v>
       </c>
       <c r="AE42" s="72">
         <f t="shared" si="157"/>
@@ -14506,7 +14506,7 @@
       </c>
       <c r="Y45" s="74">
         <f>(SUMPRODUCT(V37:V42,AD37:AD42)+SUMPRODUCT(AQ5:AQ12,AO5:AO12))/SUM(AD37:AD42,AO5:AO12)</f>
-        <v>4.4073077330908923</v>
+        <v>4.3740904222538166</v>
       </c>
       <c r="AA45" s="54" t="s">
         <v>121</v>
@@ -14667,15 +14667,15 @@
       </c>
       <c r="E49" s="28">
         <f>E50*$K$49</f>
-        <v>204.21659086121778</v>
+        <v>208.87616791028256</v>
       </c>
       <c r="F49" s="28">
         <f>F50*$K$49</f>
-        <v>2.2081782611755782</v>
+        <v>2.2585619087657482</v>
       </c>
       <c r="G49" s="28">
         <f>G50*$K$49</f>
-        <v>22.081782611755781</v>
+        <v>22.585619087657477</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>32</v>
@@ -14688,15 +14688,15 @@
       </c>
       <c r="K49" s="1">
         <f>$P$55/$O$50/(1+$E$50*$E$53+$F$50*$F$53+$G$50*$G$53)</f>
-        <v>3.4716820446407025E-2</v>
+        <v>3.5508948544748037E-2</v>
       </c>
       <c r="L49" s="28">
         <f>K49*$Y$38</f>
-        <v>1.7358410223203513E-4</v>
+        <v>1.775447427237402E-4</v>
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>3.4716820446407026</v>
+        <v>5.3263422817122059</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -14749,11 +14749,11 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="22">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="N50" s="77">
         <f>SUM(AK5:AK34,J37:J42)/K49</f>
-        <v>0.5854006628082904</v>
+        <v>0.58762591446592305</v>
       </c>
       <c r="O50" s="16">
         <f>INPUTS!O28</f>
@@ -14825,7 +14825,7 @@
       </c>
       <c r="P52" s="36">
         <f>K49+SUM(J37:J42)+SUM(AK5:AK34)</f>
-        <v>5.5040070146330104E-2</v>
+        <v>5.6374926905079017E-2</v>
       </c>
       <c r="R52" s="110"/>
       <c r="S52" s="9" t="s">
@@ -14938,7 +14938,7 @@
       </c>
       <c r="P55" s="36">
         <f t="array" ref="P55">SUM(J37:J42,AK5:AK34)+SUM(AF5:AF34*F53,L37:L42*F53)+SUM(AH5:AH34*J53,M37:M42*J53)+SUM(AE5:AE34*E53,O37:O42*E53)+SUM(N37:N42*E53,AG5:AG34*E53)</f>
-        <v>3.371971757707979E-2</v>
+        <v>3.4489094939910626E-2</v>
       </c>
       <c r="W55" s="35" t="s">
         <v>122</v>
@@ -14953,7 +14953,7 @@
       </c>
       <c r="P56" s="36">
         <f>K49+E49*E53+F49*F53+G49*G53</f>
-        <v>4.2149646971349736E-2</v>
+        <v>4.3111368674888281E-2</v>
       </c>
     </row>
     <row r="57" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15001,7 +15001,7 @@
       </c>
       <c r="P57" s="36">
         <f>P56+P55+P54</f>
-        <v>7.5869364548429519E-2</v>
+        <v>7.7600463614798915E-2</v>
       </c>
       <c r="Q57" s="32"/>
     </row>
@@ -15100,7 +15100,7 @@
       </c>
       <c r="P59" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$37:$J$42)/$P$55</f>
-        <v>0.41315381357282133</v>
+        <v>0.41050884740986027</v>
       </c>
     </row>
     <row r="60" spans="1:48" x14ac:dyDescent="0.25">
@@ -15156,7 +15156,7 @@
       </c>
       <c r="P60" s="39">
         <f>1-$K$49/$P$56</f>
-        <v>0.17634374328200197</v>
+        <v>0.17634374328200209</v>
       </c>
     </row>
     <row r="61" spans="1:48" x14ac:dyDescent="0.25">
@@ -15212,7 +15212,7 @@
       </c>
       <c r="P61" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$37:$J$42)/($P$55+N50/(1+N50)*P54)</f>
-        <v>0.41315381357282133</v>
+        <v>0.41050884740986027</v>
       </c>
     </row>
     <row r="62" spans="1:48" x14ac:dyDescent="0.25">
@@ -15268,7 +15268,7 @@
       </c>
       <c r="P62" s="39">
         <f>1-$K$49/($P$56+1/(1+N50)*P54)</f>
-        <v>0.17634374328200197</v>
+        <v>0.17634374328200209</v>
       </c>
     </row>
     <row r="64" spans="1:48" x14ac:dyDescent="0.25">
@@ -15295,7 +15295,7 @@
       </c>
       <c r="P66" s="75">
         <f>($Y$45*$P$55+$Q$50*$P$56)/($P$55+$P$56)</f>
-        <v>2.6254701035959527</v>
+        <v>2.6107068543350294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slightly reduced SSLW of first leaves.
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -1691,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:BD44"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AP8" sqref="AP8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1988,7 +1988,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="Y5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z5">
         <v>0.09</v>
@@ -3557,19 +3557,19 @@
       </c>
       <c r="J15">
         <f>P15*$U$15</f>
-        <v>4.2972599999999998E-3</v>
+        <v>4.1019300000000002E-3</v>
       </c>
       <c r="K15">
         <f>J15*0.005</f>
-        <v>2.1486299999999998E-5</v>
+        <v>2.0509650000000001E-5</v>
       </c>
       <c r="L15">
         <f>J15*$W15</f>
-        <v>1.7013068517930177</v>
+        <v>1.6239747221660625</v>
       </c>
       <c r="M15">
         <f t="shared" ref="M15:M20" si="22">J15*$X15</f>
-        <v>17.013068517930176</v>
+        <v>16.239747221660625</v>
       </c>
       <c r="N15">
         <f t="shared" ref="N15:N20" si="23">AA15*$J15</f>
@@ -3577,14 +3577,14 @@
       </c>
       <c r="O15" s="1">
         <f t="shared" ref="O15:O20" si="24">J15*$AB$16</f>
-        <v>18.958500000000001</v>
+        <v>18.09675</v>
       </c>
       <c r="P15">
         <v>1.9532999999999999E-4</v>
       </c>
       <c r="Q15" s="1">
         <f>J15*$AC15</f>
-        <v>0.24494381999999998</v>
+        <v>0.23381001000000001</v>
       </c>
       <c r="R15">
         <v>4250</v>
@@ -3596,7 +3596,7 @@
         <v>0</v>
       </c>
       <c r="U15" s="15">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V15" s="15">
         <v>4.3</v>
@@ -3628,11 +3628,11 @@
       </c>
       <c r="AD15" s="15">
         <f>J15+L15*$F$31+M15*$J$31+O15*$E$31</f>
-        <v>6.5927338413052268E-3</v>
+        <v>6.293064121245898E-3</v>
       </c>
       <c r="AE15" s="71">
         <f>(1-J15/AD15)*100</f>
-        <v>34.81823923974413</v>
+        <v>34.818239239744116</v>
       </c>
       <c r="AF15" s="1"/>
       <c r="AQ15" s="82"/>
@@ -3804,19 +3804,19 @@
       </c>
       <c r="J17">
         <f>P17*$U$17</f>
-        <v>5.3035399999999998E-3</v>
+        <v>5.0624699999999995E-3</v>
       </c>
       <c r="K17">
         <f t="shared" si="27"/>
-        <v>2.6517699999999999E-5</v>
+        <v>2.5312349999999998E-5</v>
       </c>
       <c r="L17">
         <f t="shared" ref="L17:L20" si="32">J17*$W17</f>
-        <v>2.4889358583911396</v>
+        <v>2.3758024102824513</v>
       </c>
       <c r="M17">
         <f t="shared" si="22"/>
-        <v>24.889358583911395</v>
+        <v>23.758024102824514</v>
       </c>
       <c r="N17">
         <f t="shared" si="23"/>
@@ -3824,14 +3824,14 @@
       </c>
       <c r="O17" s="1">
         <f t="shared" si="24"/>
-        <v>23.397970588235296</v>
+        <v>22.334426470588234</v>
       </c>
       <c r="P17">
         <v>2.4106999999999999E-4</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="28"/>
-        <v>0.36064071999999997</v>
+        <v>0.34424795999999996</v>
       </c>
       <c r="R17">
         <v>4250</v>
@@ -3843,7 +3843,7 @@
         <v>0</v>
       </c>
       <c r="U17" s="15">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V17" s="15">
         <v>4.8</v>
@@ -3870,11 +3870,11 @@
       </c>
       <c r="AD17" s="15">
         <f t="shared" si="30"/>
-        <v>8.5377879623382402E-3</v>
+        <v>8.1497066913228666E-3</v>
       </c>
       <c r="AE17" s="71">
         <f t="shared" si="31"/>
-        <v>37.881568113486843</v>
+        <v>37.88156811348685</v>
       </c>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
@@ -4118,19 +4118,19 @@
       </c>
       <c r="J20">
         <f>P20*$U$20</f>
-        <v>4.2242199999999999E-3</v>
+        <v>4.0322099999999996E-3</v>
       </c>
       <c r="K20">
         <f t="shared" si="27"/>
-        <v>2.11211E-5</v>
+        <v>2.0161049999999999E-5</v>
       </c>
       <c r="L20">
         <f t="shared" si="32"/>
-        <v>2.1835532433632427</v>
+        <v>2.0843008232103681</v>
       </c>
       <c r="M20">
         <f t="shared" si="22"/>
-        <v>21.835532433632427</v>
+        <v>20.843008232103678</v>
       </c>
       <c r="N20">
         <f t="shared" si="23"/>
@@ -4138,14 +4138,14 @@
       </c>
       <c r="O20" s="1">
         <f t="shared" si="24"/>
-        <v>18.636264705882354</v>
+        <v>17.789161764705881</v>
       </c>
       <c r="P20">
         <v>1.9201E-4</v>
       </c>
       <c r="Q20" s="1">
         <f t="shared" si="28"/>
-        <v>0.3168165</v>
+        <v>0.30241574999999998</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -4157,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="16">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V20" s="16">
         <v>5.0999999999999996</v>
@@ -4180,7 +4180,7 @@
       </c>
       <c r="AD20" s="16">
         <f t="shared" si="30"/>
-        <v>7.0076137152537141E-3</v>
+        <v>6.689085819105817E-3</v>
       </c>
       <c r="AE20" s="72">
         <f t="shared" si="31"/>
@@ -4252,7 +4252,7 @@
       </c>
       <c r="Y23" s="74">
         <f>(SUMPRODUCT(V15:V20,AD15:AD20)+SUMPRODUCT(AS5:AS12,AQ5:AQ12))/SUM(AD15:AD20,AQ5:AQ12)</f>
-        <v>4.4146203981518433</v>
+        <v>4.4039658411029281</v>
       </c>
       <c r="AA23" s="54" t="s">
         <v>121</v>
@@ -4414,15 +4414,15 @@
       </c>
       <c r="E27" s="28">
         <f>E28*$K$27</f>
-        <v>154.21320252380491</v>
+        <v>149.46818795927152</v>
       </c>
       <c r="F27" s="28">
         <f>F28*$K$27</f>
-        <v>2.0990033143932734</v>
+        <v>2.0344186930067711</v>
       </c>
       <c r="G27" s="28">
         <f>G28*$K$27</f>
-        <v>20.990033143932731</v>
+        <v>20.344186930067711</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>32</v>
@@ -4435,15 +4435,15 @@
       </c>
       <c r="K27" s="1">
         <f>$P$33/$O$28/(1+$E$28*$E$31+$F$28*$F$31+$G$28*$G$31)</f>
-        <v>3.4954992572062443E-2</v>
+        <v>3.3879455937434876E-2</v>
       </c>
       <c r="L27" s="28">
         <f>K27*$Y$16</f>
-        <v>1.7477496286031222E-4</v>
+        <v>1.6939727968717439E-4</v>
       </c>
       <c r="M27" s="28">
         <f>M28*$K$27</f>
-        <v>2.7963994057649955</v>
+        <v>2.7103564749947902</v>
       </c>
       <c r="N27" s="76" t="s">
         <v>134</v>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="N28" s="77">
         <f>SUM(AK5:AK12,J15:J20)/K27</f>
-        <v>0.59334451961947088</v>
+        <v>0.59363241585441173</v>
       </c>
       <c r="O28" s="16">
         <v>0.8</v>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="P30" s="69">
         <f>K27+SUM(J15:J20)+SUM(AK5:AK12)</f>
-        <v>5.5695345848035004E-2</v>
+        <v>5.3991399213407433E-2</v>
       </c>
       <c r="R30" s="112"/>
       <c r="S30" s="9" t="s">
@@ -4687,7 +4687,7 @@
       </c>
       <c r="P33" s="69">
         <f t="array" ref="P33">SUM(J15:J20,AK5:AK12)+SUM(AF5:AF12*F31,L15:L20*F31)+SUM(AH5:AH12*J31,M15:M20*J31)+SUM(AE5:AE12*E31,O15:O20*E31)+SUM(N15:N20*E31,AG5:AG12*E31)</f>
-        <v>3.2704112436364279E-2</v>
+        <v>3.1697833549141685E-2</v>
       </c>
       <c r="W33" s="35" t="s">
         <v>122</v>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="P34" s="36">
         <f>K27+E27*E31+F27*F31+G27*G31</f>
-        <v>4.0880140545455336E-2</v>
+        <v>3.9622291936427113E-2</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4750,7 +4750,7 @@
       </c>
       <c r="P35" s="36">
         <f>P34+P33+P32</f>
-        <v>7.3584252981819614E-2</v>
+        <v>7.1320125485568792E-2</v>
       </c>
       <c r="Q35" s="32"/>
     </row>
@@ -4802,7 +4802,7 @@
       </c>
       <c r="P37" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$15:$J$20)/$P$33</f>
-        <v>0.36581818826824364</v>
+        <v>0.36551047740241704</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -4811,7 +4811,7 @@
       </c>
       <c r="P38" s="39">
         <f>1-$K$27/$P$34</f>
-        <v>0.14493952061648663</v>
+        <v>0.14493952061648685</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -4820,7 +4820,7 @@
       </c>
       <c r="P39" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$15:$J$20)/($P$33+N28/(1+N28)*P32)</f>
-        <v>0.36581818826824364</v>
+        <v>0.36551047740241704</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -4829,7 +4829,7 @@
       </c>
       <c r="P40" s="39">
         <f>1-$K$27/($P$34+1/(1+N28)*P32)</f>
-        <v>0.14493952061648663</v>
+        <v>0.14493952061648685</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="P44" s="75">
         <f>($Y$23*$P$33+$Q$28*$P$34)/($P$33+$P$34)</f>
-        <v>2.6287201769563748</v>
+        <v>2.6239848182679681</v>
       </c>
     </row>
   </sheetData>
@@ -7704,8 +7704,8 @@
   </sheetPr>
   <dimension ref="A1:BD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AM32" sqref="AM32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7990,8 +7990,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="Y5">
-        <f>INPUTS!Y5</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z5">
         <f>INPUTS!Z5</f>
@@ -14005,19 +14004,19 @@
       </c>
       <c r="J37">
         <f>P37*$U$37</f>
-        <v>4.3023282082452321E-3</v>
+        <v>4.1067678351431759E-3</v>
       </c>
       <c r="K37">
         <f>J37*0.005</f>
-        <v>2.1511641041226162E-5</v>
+        <v>2.053383917571588E-5</v>
       </c>
       <c r="L37">
         <f>J37*$W37</f>
-        <v>1.7741886232211572</v>
+        <v>1.6935436858020134</v>
       </c>
       <c r="M37">
         <f t="shared" ref="M37:M42" si="149">J37*$X37</f>
-        <v>17.74188623221157</v>
+        <v>16.935436858020136</v>
       </c>
       <c r="N37">
         <f t="shared" ref="N37:N42" si="150">AA37*$J37</f>
@@ -14025,14 +14024,14 @@
       </c>
       <c r="O37" s="1">
         <f t="shared" ref="O37:O42" si="151">J37*$AB$38</f>
-        <v>25.307812989677835</v>
+        <v>24.157457853783384</v>
       </c>
       <c r="P37">
         <v>1.9556037310205601E-4</v>
       </c>
       <c r="Q37" s="1">
         <f t="shared" ref="Q37:Q42" si="152">J37*$AC37</f>
-        <v>0.36569789770084471</v>
+        <v>0.34907526598716992</v>
       </c>
       <c r="R37">
         <v>4400</v>
@@ -14045,7 +14044,7 @@
       </c>
       <c r="U37" s="15">
         <f>INPUTS!U15</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V37" s="15">
         <f>INPUTS!V15</f>
@@ -14078,7 +14077,7 @@
       </c>
       <c r="AD37" s="15">
         <f>J37+L37*$F$53+M37*$J$53+O37*$E$53</f>
-        <v>6.8543416050531256E-3</v>
+        <v>6.5427806230052557E-3</v>
       </c>
       <c r="AE37" s="71">
         <f>(1-J37/AD37)*100</f>
@@ -14258,19 +14257,19 @@
       </c>
       <c r="J39">
         <f>P39*$U$39</f>
-        <v>5.0680069287428898E-3</v>
+        <v>4.8376429774363953E-3</v>
       </c>
       <c r="K39">
         <f t="shared" si="156"/>
-        <v>2.5340034643714449E-5</v>
+        <v>2.4188214887181978E-5</v>
       </c>
       <c r="L39">
         <f t="shared" ref="L39:L42" si="159">J39*$W39</f>
-        <v>2.4761936124967816</v>
+        <v>2.3636393573832919</v>
       </c>
       <c r="M39">
         <f t="shared" si="149"/>
-        <v>24.761936124967814</v>
+        <v>23.636393573832915</v>
       </c>
       <c r="N39">
         <f t="shared" si="150"/>
@@ -14278,14 +14277,14 @@
       </c>
       <c r="O39" s="1">
         <f t="shared" si="151"/>
-        <v>29.811805463193469</v>
+        <v>28.456723396684676</v>
       </c>
       <c r="P39">
         <v>2.3036395130649501E-4</v>
       </c>
       <c r="Q39" s="1">
         <f t="shared" si="152"/>
-        <v>0.51186869980303185</v>
+        <v>0.48860194072107593</v>
       </c>
       <c r="R39">
         <v>4400</v>
@@ -14298,7 +14297,7 @@
       </c>
       <c r="U39" s="15">
         <f>INPUTS!U17</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V39" s="15">
         <f>INPUTS!V17</f>
@@ -14326,11 +14325,11 @@
       </c>
       <c r="AD39" s="15">
         <f t="shared" si="157"/>
-        <v>8.4723718951712264E-3</v>
+        <v>8.0872640817543518E-3</v>
       </c>
       <c r="AE39" s="71">
         <f t="shared" si="158"/>
-        <v>40.181958589053821</v>
+        <v>40.181958589053814</v>
       </c>
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
@@ -14578,19 +14577,19 @@
       </c>
       <c r="J42">
         <f>P42*$U$42</f>
-        <v>4.3694199999999997E-3</v>
+        <v>4.1708099999999996E-3</v>
       </c>
       <c r="K42">
         <f t="shared" si="156"/>
-        <v>2.18471E-5</v>
+        <v>2.0854049999999997E-5</v>
       </c>
       <c r="L42">
         <f t="shared" si="159"/>
-        <v>2.3509226953550577</v>
+        <v>2.2440625728389185</v>
       </c>
       <c r="M42">
         <f t="shared" si="149"/>
-        <v>23.509226953550574</v>
+        <v>22.440625728389183</v>
       </c>
       <c r="N42">
         <f t="shared" si="150"/>
@@ -14598,14 +14597,14 @@
       </c>
       <c r="O42" s="1">
         <f t="shared" si="151"/>
-        <v>25.70247058823529</v>
+        <v>24.534176470588232</v>
       </c>
       <c r="P42">
         <v>1.9861E-4</v>
       </c>
       <c r="Q42" s="1">
         <f t="shared" si="152"/>
-        <v>0.48500561999999997</v>
+        <v>0.46295990999999997</v>
       </c>
       <c r="R42">
         <f>INPUTS!R20</f>
@@ -14619,7 +14618,7 @@
       </c>
       <c r="U42" s="16">
         <f>INPUTS!U20</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V42" s="16">
         <f>INPUTS!V20</f>
@@ -14643,7 +14642,7 @@
       </c>
       <c r="AD42" s="16">
         <f t="shared" si="157"/>
-        <v>7.5272391193074283E-3</v>
+        <v>7.1850918866116359E-3</v>
       </c>
       <c r="AE42" s="72">
         <f t="shared" si="158"/>
@@ -14718,7 +14717,7 @@
       </c>
       <c r="Y45" s="74">
         <f>(SUMPRODUCT(V37:V42,AD37:AD42)+SUMPRODUCT(AR5:AR12,AP5:AP12))/SUM(AD37:AD42,AP5:AP12)</f>
-        <v>4.3740904222538166</v>
+        <v>4.3619109572720793</v>
       </c>
       <c r="AA45" s="54" t="s">
         <v>121</v>
@@ -14883,15 +14882,15 @@
       </c>
       <c r="E49" s="28">
         <f>E50*$K$49</f>
-        <v>208.87616791028256</v>
+        <v>202.5847905487137</v>
       </c>
       <c r="F49" s="28">
         <f>F50*$K$49</f>
-        <v>2.2585619087657482</v>
+        <v>2.1905337301340246</v>
       </c>
       <c r="G49" s="28">
         <f>G50*$K$49</f>
-        <v>22.585619087657477</v>
+        <v>21.905337301340243</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>32</v>
@@ -14904,15 +14903,15 @@
       </c>
       <c r="K49" s="1">
         <f>$P$55/$O$50/(1+$E$50*$E$53+$F$50*$F$53+$G$50*$G$53)</f>
-        <v>3.5508948544748037E-2</v>
+        <v>3.4439414393281333E-2</v>
       </c>
       <c r="L49" s="28">
         <f>K49*$Y$38</f>
-        <v>1.775447427237402E-4</v>
+        <v>1.7219707196640668E-4</v>
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>5.3263422817122059</v>
+        <v>5.1659121589921995</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -14970,7 +14969,7 @@
       </c>
       <c r="N50" s="77">
         <f>SUM(AK5:AK34,J37:J42)/K49</f>
-        <v>0.58762591446592305</v>
+        <v>0.58774065681765075</v>
       </c>
       <c r="O50" s="16">
         <f>INPUTS!O28</f>
@@ -15044,7 +15043,7 @@
       </c>
       <c r="P52" s="36">
         <f>K49+SUM(J37:J42)+SUM(AK5:AK34)</f>
-        <v>5.6374926905079017E-2</v>
+        <v>5.4680858429203755E-2</v>
       </c>
       <c r="R52" s="112"/>
       <c r="S52" s="9" t="s">
@@ -15159,7 +15158,7 @@
       </c>
       <c r="P55" s="36">
         <f t="array" ref="P55">SUM(J37:J42,AK5:AK34)+SUM(AF5:AF34*F53,L37:L42*F53)+SUM(AH5:AH34*J53,M37:M42*J53)+SUM(AE5:AE34*E53,O37:O42*E53)+SUM(N37:N42*E53,AG5:AG34*E53)</f>
-        <v>3.4489094939910626E-2</v>
+        <v>3.3450278911750092E-2</v>
       </c>
       <c r="W55" s="35" t="s">
         <v>122</v>
@@ -15174,7 +15173,7 @@
       </c>
       <c r="P56" s="36">
         <f>K49+E49*E53+F49*F53+G49*G53</f>
-        <v>4.3111368674888281E-2</v>
+        <v>4.1812848639687608E-2</v>
       </c>
     </row>
     <row r="57" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15222,7 +15221,7 @@
       </c>
       <c r="P57" s="36">
         <f>P56+P55+P54</f>
-        <v>7.7600463614798915E-2</v>
+        <v>7.52631275514377E-2</v>
       </c>
       <c r="Q57" s="32"/>
     </row>
@@ -15321,7 +15320,7 @@
       </c>
       <c r="P59" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$37:$J$42)/$P$55</f>
-        <v>0.41050884740986027</v>
+        <v>0.41087241587729117</v>
       </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.25">
@@ -15377,7 +15376,7 @@
       </c>
       <c r="P60" s="39">
         <f>1-$K$49/$P$56</f>
-        <v>0.17634374328200209</v>
+        <v>0.17634374328200197</v>
       </c>
     </row>
     <row r="61" spans="1:49" x14ac:dyDescent="0.25">
@@ -15433,7 +15432,7 @@
       </c>
       <c r="P61" s="39">
         <f>1-SUM($AK$5:$AK$12,$J$37:$J$42)/($P$55+N50/(1+N50)*P54)</f>
-        <v>0.41050884740986027</v>
+        <v>0.41087241587729117</v>
       </c>
     </row>
     <row r="62" spans="1:49" x14ac:dyDescent="0.25">
@@ -15489,7 +15488,7 @@
       </c>
       <c r="P62" s="39">
         <f>1-$K$49/($P$56+1/(1+N50)*P54)</f>
-        <v>0.17634374328200209</v>
+        <v>0.17634374328200197</v>
       </c>
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.25">
@@ -15516,7 +15515,7 @@
       </c>
       <c r="P66" s="75">
         <f>($Y$45*$P$55+$Q$50*$P$56)/($P$55+$P$56)</f>
-        <v>2.6107068543350294</v>
+        <v>2.6052937587875906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change initial value of integral_conc_sucrose_em_prec
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS" sheetId="15" r:id="rId1"/>
@@ -1691,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:BD44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO21" sqref="AO21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2049,7 @@
         <v>2100</v>
       </c>
       <c r="AP5" s="1">
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AQ5" s="70">
         <f>AK5+AE5*$E$31+AF5*$F$31+AH5*$J$31</f>
@@ -2239,7 +2239,7 @@
         <v>2100</v>
       </c>
       <c r="AP6" s="1">
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AQ6" s="70">
         <f t="shared" ref="AQ6:AQ12" si="16">AK6+AE6*$E$31+AF6*$F$31+AH6*$J$31</f>
@@ -2428,7 +2428,7 @@
         <v>2100</v>
       </c>
       <c r="AP7" s="1">
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AQ7" s="70">
         <f t="shared" si="16"/>
@@ -7704,8 +7704,8 @@
   </sheetPr>
   <dimension ref="A1:BD66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AJ15" sqref="AJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8050,7 +8050,7 @@
       </c>
       <c r="AO5">
         <f>INPUTS!AP5</f>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP5" s="70">
         <f t="shared" ref="AP5:AP34" si="4">AK5+(AE5+AG5)*$E$53+AF5*$F$53+AH5*$J$53</f>
@@ -8243,7 +8243,7 @@
       </c>
       <c r="AO6">
         <f>INPUTS!AP6</f>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP6" s="70">
         <f t="shared" si="4"/>
@@ -8435,7 +8435,7 @@
       </c>
       <c r="AO7">
         <f>INPUTS!AP7</f>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP7" s="70">
         <f t="shared" si="4"/>
@@ -9599,7 +9599,7 @@
       </c>
       <c r="AO13">
         <f t="shared" ref="AO13:AO34" si="24">AO6</f>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP13" s="70">
         <f t="shared" si="4"/>
@@ -9799,7 +9799,7 @@
       </c>
       <c r="AO14">
         <f t="shared" si="24"/>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP14" s="70">
         <f t="shared" si="4"/>
@@ -11005,7 +11005,7 @@
       </c>
       <c r="AO20">
         <f t="shared" si="24"/>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP20" s="70">
         <f t="shared" si="4"/>
@@ -11206,7 +11206,7 @@
       </c>
       <c r="AO21">
         <f t="shared" si="24"/>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP21" s="70">
         <f t="shared" si="4"/>
@@ -12412,7 +12412,7 @@
       </c>
       <c r="AO27">
         <f t="shared" si="24"/>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP27" s="70">
         <f t="shared" si="4"/>
@@ -12613,7 +12613,7 @@
       </c>
       <c r="AO28">
         <f t="shared" si="24"/>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP28" s="70">
         <f t="shared" si="4"/>
@@ -13819,7 +13819,7 @@
       </c>
       <c r="AO34">
         <f t="shared" si="24"/>
-        <v>1450</v>
+        <v>1800</v>
       </c>
       <c r="AP34" s="73">
         <f t="shared" si="4"/>
@@ -18238,7 +18238,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correction age of first leaves
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS" sheetId="15" r:id="rId1"/>
@@ -1691,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:BD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO21" sqref="AO21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,8 +3546,7 @@
         <v>39</v>
       </c>
       <c r="G15" s="48">
-        <f>280</f>
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="H15" s="48">
         <v>8.2000000000000003E-2</v>
@@ -3669,8 +3668,8 @@
         <v>41</v>
       </c>
       <c r="G16" s="48">
-        <f>280</f>
-        <v>280</v>
+        <f>80+G17</f>
+        <v>220</v>
       </c>
       <c r="H16" s="48">
         <v>2.8500000000000001E-2</v>
@@ -3794,7 +3793,7 @@
         <v>39</v>
       </c>
       <c r="G17" s="48">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="H17" s="48">
         <v>9.1999999999999998E-2</v>
@@ -3897,7 +3896,7 @@
         <v>42</v>
       </c>
       <c r="G18" s="48">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="H18" s="48">
         <v>2.8500000000000001E-2</v>
@@ -4000,7 +3999,8 @@
         <v>41</v>
       </c>
       <c r="G19" s="48">
-        <v>180</v>
+        <f>80+G20</f>
+        <v>140</v>
       </c>
       <c r="H19" s="48">
         <v>5.0000000000000001E-4</v>
@@ -4108,7 +4108,7 @@
         <v>39</v>
       </c>
       <c r="G20" s="48">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="H20" s="48">
         <v>6.0421565000000003E-2</v>
@@ -7704,8 +7704,8 @@
   </sheetPr>
   <dimension ref="A1:BD66"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AJ15" sqref="AJ15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13993,8 +13993,8 @@
         <v>39</v>
       </c>
       <c r="G37" s="48">
-        <f>280</f>
-        <v>280</v>
+        <f>INPUTS!G15</f>
+        <v>220</v>
       </c>
       <c r="H37" s="48">
         <v>8.2000000000000003E-2</v>
@@ -14119,8 +14119,8 @@
         <v>41</v>
       </c>
       <c r="G38" s="48">
-        <f>280</f>
-        <v>280</v>
+        <f>INPUTS!G16</f>
+        <v>220</v>
       </c>
       <c r="H38" s="48">
         <v>2.8500000000000001E-2</v>
@@ -14247,7 +14247,8 @@
         <v>39</v>
       </c>
       <c r="G39" s="48">
-        <v>180</v>
+        <f>INPUTS!G17</f>
+        <v>140</v>
       </c>
       <c r="H39" s="48">
         <v>9.1999999999999998E-2</v>
@@ -14352,7 +14353,8 @@
         <v>42</v>
       </c>
       <c r="G40" s="48">
-        <v>180</v>
+        <f>INPUTS!G18</f>
+        <v>140</v>
       </c>
       <c r="H40" s="48">
         <v>2.8500000000000001E-2</v>
@@ -14457,7 +14459,8 @@
         <v>41</v>
       </c>
       <c r="G41" s="48">
-        <v>180</v>
+        <f>INPUTS!G19</f>
+        <v>140</v>
       </c>
       <c r="H41" s="48">
         <v>5.0000000000000001E-4</v>
@@ -14567,7 +14570,8 @@
         <v>39</v>
       </c>
       <c r="G42" s="48">
-        <v>80</v>
+        <f>INPUTS!G20</f>
+        <v>60</v>
       </c>
       <c r="H42" s="48">
         <v>6.0421565000000003E-2</v>

</xml_diff>

<commit_message>
- change inputs to delay senescence of leaves 1 to 3 - add some charts
</commit_message>
<xml_diff>
--- a/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/tillering_hack/fspmwheat/inputs/Generate_inputs.xlsx
@@ -1691,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:BD44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,7 +3546,8 @@
         <v>39</v>
       </c>
       <c r="G15" s="48">
-        <v>220</v>
+        <f>G16</f>
+        <v>240</v>
       </c>
       <c r="H15" s="48">
         <v>8.2000000000000003E-2</v>
@@ -3669,7 +3670,7 @@
       </c>
       <c r="G16" s="48">
         <f>80+G17</f>
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="H16" s="48">
         <v>2.8500000000000001E-2</v>
@@ -3793,7 +3794,8 @@
         <v>39</v>
       </c>
       <c r="G17" s="48">
-        <v>140</v>
+        <f>G19</f>
+        <v>160</v>
       </c>
       <c r="H17" s="48">
         <v>9.1999999999999998E-2</v>
@@ -3829,7 +3831,7 @@
         <v>2.4106999999999999E-4</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" si="28"/>
+        <f>J17*$AC17</f>
         <v>0.34424795999999996</v>
       </c>
       <c r="R17">
@@ -3896,7 +3898,8 @@
         <v>42</v>
       </c>
       <c r="G18" s="48">
-        <v>140</v>
+        <f>G19</f>
+        <v>160</v>
       </c>
       <c r="H18" s="48">
         <v>2.8500000000000001E-2</v>
@@ -4000,7 +4003,7 @@
       </c>
       <c r="G19" s="48">
         <f>80+G20</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H19" s="48">
         <v>5.0000000000000001E-4</v>
@@ -4107,8 +4110,8 @@
       <c r="F20" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="48">
-        <v>60</v>
+      <c r="G20" s="46">
+        <v>80</v>
       </c>
       <c r="H20" s="48">
         <v>6.0421565000000003E-2</v>
@@ -4443,7 +4446,7 @@
       </c>
       <c r="M27" s="28">
         <f>M28*$K$27</f>
-        <v>2.7103564749947902</v>
+        <v>8.4698639843587191</v>
       </c>
       <c r="N27" s="76" t="s">
         <v>134</v>
@@ -4497,7 +4500,7 @@
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
       <c r="M28" s="22">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="N28" s="77">
         <f>SUM(AK5:AK12,J15:J20)/K27</f>
@@ -7705,7 +7708,7 @@
   <dimension ref="A1:BD66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13994,7 +13997,7 @@
       </c>
       <c r="G37" s="48">
         <f>INPUTS!G15</f>
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="H37" s="48">
         <v>8.2000000000000003E-2</v>
@@ -14120,7 +14123,7 @@
       </c>
       <c r="G38" s="48">
         <f>INPUTS!G16</f>
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="H38" s="48">
         <v>2.8500000000000001E-2</v>
@@ -14248,7 +14251,7 @@
       </c>
       <c r="G39" s="48">
         <f>INPUTS!G17</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H39" s="48">
         <v>9.1999999999999998E-2</v>
@@ -14354,7 +14357,7 @@
       </c>
       <c r="G40" s="48">
         <f>INPUTS!G18</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H40" s="48">
         <v>2.8500000000000001E-2</v>
@@ -14460,7 +14463,7 @@
       </c>
       <c r="G41" s="48">
         <f>INPUTS!G19</f>
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="H41" s="48">
         <v>5.0000000000000001E-4</v>
@@ -14571,7 +14574,7 @@
       </c>
       <c r="G42" s="48">
         <f>INPUTS!G20</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H42" s="48">
         <v>6.0421565000000003E-2</v>
@@ -14915,7 +14918,7 @@
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>5.1659121589921995</v>
+        <v>8.609853598320333</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -14969,7 +14972,8 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="22">
-        <v>150</v>
+        <f>INPUTS!M28</f>
+        <v>250</v>
       </c>
       <c r="N50" s="77">
         <f>SUM(AK5:AK34,J37:J42)/K49</f>

</xml_diff>